<commit_message>
feat: mejoras en movilidades y diálogos de expedientes
- Cambiar diálogo de expedientes a formato panorámico (75vw x 70vh)
- Eliminar botón X de cierre, mantener cierre al hacer clic afuera
- Arreglar scroll para que no rompa esquinas redondeadas del diálogo
- Eliminar rendimiento de combustible de tickets
- Agregar nueva pestaña de Historial Mecánico con CRUD completo
- Agregar lista de personas habilitadas por vehículo
- Cambiar Badge por texto normal en campos tipo/categoría de diálogos
- Actualizar tipos de vehículos: reemplazar Moto por Máquina
- Agregar text-white a todos los botones azules en Movilidades
</commit_message>
<xml_diff>
--- a/src-tauri/resources/templates/MODELO_ORDEN_DE_COMPRA.xlsx
+++ b/src-tauri/resources/templates/MODELO_ORDEN_DE_COMPRA.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauti\Desktop\Proyectos\GestorExpedientesV2\gestor-irrigacion\src-tauri\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFDEC09-C134-40D1-8398-89C5BDDE0996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4FEDF-21B5-4A4C-B68E-8719A76DB826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01 OK" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -509,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -637,6 +637,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -657,8 +660,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1536,7 +1539,7 @@
   </sheetPr>
   <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -1574,7 +1577,7 @@
       <c r="E2" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="72"/>
       <c r="G2" s="55"/>
     </row>
     <row r="3" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
@@ -1704,33 +1707,33 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="71" t="s">
+      <c r="A15" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="71"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="71"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="51" t="s">
@@ -1753,42 +1756,42 @@
       <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="65"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="66"/>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="48"/>
@@ -1903,15 +1906,15 @@
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="31"/>
@@ -1925,11 +1928,11 @@
     <row r="35" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="27"/>
       <c r="B35" s="27"/>
-      <c r="C35" s="68" t="s">
+      <c r="C35" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="69"/>
-      <c r="E35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="71"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
@@ -2264,33 +2267,33 @@
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="71" t="s">
+      <c r="A66" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B66" s="71"/>
-      <c r="C66" s="71"/>
-      <c r="D66" s="71"/>
-      <c r="E66" s="71"/>
-      <c r="F66" s="71"/>
-      <c r="G66" s="71"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="64"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="71"/>
-      <c r="B67" s="71"/>
-      <c r="C67" s="71"/>
-      <c r="D67" s="71"/>
-      <c r="E67" s="71"/>
-      <c r="F67" s="71"/>
-      <c r="G67" s="71"/>
+      <c r="A67" s="64"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="64"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" s="71"/>
-      <c r="B68" s="71"/>
-      <c r="C68" s="71"/>
-      <c r="D68" s="71"/>
-      <c r="E68" s="71"/>
-      <c r="F68" s="71"/>
-      <c r="G68" s="71"/>
+      <c r="A68" s="64"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="64"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="51" t="s">
@@ -2313,42 +2316,42 @@
       <c r="G70" s="49"/>
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="64" t="s">
+      <c r="A71" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B71" s="64"/>
-      <c r="C71" s="64"/>
-      <c r="D71" s="64"/>
-      <c r="E71" s="64"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="64"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="65"/>
+      <c r="D71" s="65"/>
+      <c r="E71" s="65"/>
+      <c r="F71" s="65"/>
+      <c r="G71" s="65"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" s="65"/>
-      <c r="B72" s="65"/>
-      <c r="C72" s="65"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
+      <c r="A72" s="66"/>
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="65"/>
-      <c r="B73" s="65"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
+      <c r="A73" s="66"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="66"/>
-      <c r="B74" s="66"/>
-      <c r="C74" s="66"/>
-      <c r="D74" s="66"/>
-      <c r="E74" s="66"/>
-      <c r="F74" s="66"/>
-      <c r="G74" s="66"/>
+      <c r="A74" s="67"/>
+      <c r="B74" s="67"/>
+      <c r="C74" s="67"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="67"/>
+      <c r="F74" s="67"/>
+      <c r="G74" s="67"/>
     </row>
     <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="48"/>
@@ -2380,7 +2383,7 @@
       </c>
       <c r="G76" s="4"/>
     </row>
-    <row r="77" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="45">
         <v>1</v>
       </c>
@@ -2483,15 +2486,15 @@
       <c r="H83" s="61"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A84" s="67" t="s">
+      <c r="A84" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="67"/>
-      <c r="C84" s="67"/>
-      <c r="D84" s="67"/>
-      <c r="E84" s="67"/>
-      <c r="F84" s="67"/>
-      <c r="G84" s="67"/>
+      <c r="B84" s="68"/>
+      <c r="C84" s="68"/>
+      <c r="D84" s="68"/>
+      <c r="E84" s="68"/>
+      <c r="F84" s="68"/>
+      <c r="G84" s="68"/>
       <c r="H84" s="61"/>
     </row>
     <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2507,11 +2510,11 @@
     <row r="86" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="27"/>
       <c r="B86" s="27"/>
-      <c r="C86" s="68" t="s">
+      <c r="C86" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D86" s="69"/>
-      <c r="E86" s="70"/>
+      <c r="D86" s="70"/>
+      <c r="E86" s="71"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="61"/>
@@ -2831,33 +2834,33 @@
       <c r="G113" s="4"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="71" t="s">
+      <c r="A114" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B114" s="71"/>
-      <c r="C114" s="71"/>
-      <c r="D114" s="71"/>
-      <c r="E114" s="71"/>
-      <c r="F114" s="71"/>
-      <c r="G114" s="71"/>
+      <c r="B114" s="64"/>
+      <c r="C114" s="64"/>
+      <c r="D114" s="64"/>
+      <c r="E114" s="64"/>
+      <c r="F114" s="64"/>
+      <c r="G114" s="64"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="71"/>
-      <c r="B115" s="71"/>
-      <c r="C115" s="71"/>
-      <c r="D115" s="71"/>
-      <c r="E115" s="71"/>
-      <c r="F115" s="71"/>
-      <c r="G115" s="71"/>
+      <c r="A115" s="64"/>
+      <c r="B115" s="64"/>
+      <c r="C115" s="64"/>
+      <c r="D115" s="64"/>
+      <c r="E115" s="64"/>
+      <c r="F115" s="64"/>
+      <c r="G115" s="64"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A116" s="71"/>
-      <c r="B116" s="71"/>
-      <c r="C116" s="71"/>
-      <c r="D116" s="71"/>
-      <c r="E116" s="71"/>
-      <c r="F116" s="71"/>
-      <c r="G116" s="71"/>
+      <c r="A116" s="64"/>
+      <c r="B116" s="64"/>
+      <c r="C116" s="64"/>
+      <c r="D116" s="64"/>
+      <c r="E116" s="64"/>
+      <c r="F116" s="64"/>
+      <c r="G116" s="64"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="51" t="s">
@@ -2880,42 +2883,42 @@
       <c r="G118" s="49"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A119" s="64" t="s">
+      <c r="A119" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B119" s="64"/>
-      <c r="C119" s="64"/>
-      <c r="D119" s="64"/>
-      <c r="E119" s="64"/>
-      <c r="F119" s="64"/>
-      <c r="G119" s="64"/>
+      <c r="B119" s="65"/>
+      <c r="C119" s="65"/>
+      <c r="D119" s="65"/>
+      <c r="E119" s="65"/>
+      <c r="F119" s="65"/>
+      <c r="G119" s="65"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="65"/>
-      <c r="B120" s="65"/>
-      <c r="C120" s="65"/>
-      <c r="D120" s="65"/>
-      <c r="E120" s="65"/>
-      <c r="F120" s="65"/>
-      <c r="G120" s="65"/>
+      <c r="A120" s="66"/>
+      <c r="B120" s="66"/>
+      <c r="C120" s="66"/>
+      <c r="D120" s="66"/>
+      <c r="E120" s="66"/>
+      <c r="F120" s="66"/>
+      <c r="G120" s="66"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="65"/>
-      <c r="B121" s="65"/>
-      <c r="C121" s="65"/>
-      <c r="D121" s="65"/>
-      <c r="E121" s="65"/>
-      <c r="F121" s="65"/>
-      <c r="G121" s="65"/>
+      <c r="A121" s="66"/>
+      <c r="B121" s="66"/>
+      <c r="C121" s="66"/>
+      <c r="D121" s="66"/>
+      <c r="E121" s="66"/>
+      <c r="F121" s="66"/>
+      <c r="G121" s="66"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A122" s="66"/>
-      <c r="B122" s="66"/>
-      <c r="C122" s="66"/>
-      <c r="D122" s="66"/>
-      <c r="E122" s="66"/>
-      <c r="F122" s="66"/>
-      <c r="G122" s="66"/>
+      <c r="A122" s="67"/>
+      <c r="B122" s="67"/>
+      <c r="C122" s="67"/>
+      <c r="D122" s="67"/>
+      <c r="E122" s="67"/>
+      <c r="F122" s="67"/>
+      <c r="G122" s="67"/>
     </row>
     <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="48"/>
@@ -2947,7 +2950,7 @@
       </c>
       <c r="G124" s="4"/>
     </row>
-    <row r="125" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A125" s="45">
         <v>1</v>
       </c>
@@ -3043,15 +3046,15 @@
       <c r="G131" s="4"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A132" s="67" t="s">
+      <c r="A132" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B132" s="67"/>
-      <c r="C132" s="67"/>
-      <c r="D132" s="67"/>
-      <c r="E132" s="67"/>
-      <c r="F132" s="67"/>
-      <c r="G132" s="67"/>
+      <c r="B132" s="68"/>
+      <c r="C132" s="68"/>
+      <c r="D132" s="68"/>
+      <c r="E132" s="68"/>
+      <c r="F132" s="68"/>
+      <c r="G132" s="68"/>
     </row>
     <row r="133" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A133" s="31"/>
@@ -3065,11 +3068,11 @@
     <row r="134" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A134" s="27"/>
       <c r="B134" s="27"/>
-      <c r="C134" s="68" t="s">
+      <c r="C134" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D134" s="69"/>
-      <c r="E134" s="70"/>
+      <c r="D134" s="70"/>
+      <c r="E134" s="71"/>
       <c r="F134" s="4"/>
       <c r="G134" s="4"/>
     </row>
@@ -3209,11 +3212,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A15:G17"/>
-    <mergeCell ref="A20:G23"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="A66:G68"/>
     <mergeCell ref="A119:G122"/>
     <mergeCell ref="A132:G132"/>
     <mergeCell ref="C134:E134"/>
@@ -3221,6 +3219,11 @@
     <mergeCell ref="A84:G84"/>
     <mergeCell ref="C86:E86"/>
     <mergeCell ref="A114:G116"/>
+    <mergeCell ref="A15:G17"/>
+    <mergeCell ref="A20:G23"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="A66:G68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" r:id="rId1"/>

</xml_diff>